<commit_message>
Included Mixed Logit Model
</commit_message>
<xml_diff>
--- a/MILP/Input Data/master_problem_inputs_with_taste_draws.xlsx
+++ b/MILP/Input Data/master_problem_inputs_with_taste_draws.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atfan\OneDrive\Desktop\M.Sc DDS\Sem 4\Master's Thesis\Code\MILP\Input Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atfan\Desktop\M.Sc DDS\Sem 4\Master's Thesis\Code\MILP\Input Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC823787-4F47-44C3-BE9C-A439C43BDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48741B5A-EE4D-494C-AF71-A3793FC347E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD_pairs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="53">
   <si>
     <t>origin_id</t>
   </si>
@@ -193,6 +193,12 @@
   <si>
     <t>taste_draw_count_R</t>
   </si>
+  <si>
+    <t>0.10972690781987848</t>
+  </si>
+  <si>
+    <t>0.016649426669571643</t>
+  </si>
 </sst>
 </file>
 
@@ -250,11 +256,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1707,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M194" sqref="M194"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,16 +1763,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D2">
-        <v>-0.2359</v>
+        <v>-0.33238680375983398</v>
       </c>
       <c r="E2">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7841142560871403E-2</v>
       </c>
       <c r="F2">
         <v>0.80410000000000004</v>
       </c>
       <c r="G2">
-        <v>0.15820000000000001</v>
+        <v>0.27838088829549701</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1779,16 +1786,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-0.2359</v>
+        <v>-0.33238680375983398</v>
       </c>
       <c r="E3">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7841142560871403E-2</v>
       </c>
       <c r="F3">
         <v>0.80410000000000004</v>
       </c>
       <c r="G3">
-        <v>0.15820000000000001</v>
+        <v>0.27838088829549701</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1802,16 +1809,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D4">
-        <v>-0.2359</v>
+        <v>-0.17653148635790999</v>
       </c>
       <c r="E4">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.0598944969622297E-2</v>
       </c>
       <c r="F4">
         <v>0.80410000000000004</v>
       </c>
       <c r="G4">
-        <v>0.15820000000000001</v>
+        <v>0.19117356776814501</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1825,16 +1832,16 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-0.2359</v>
+        <v>-0.17653148635790999</v>
       </c>
       <c r="E5">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.0598944969622297E-2</v>
       </c>
       <c r="F5">
         <v>0.80410000000000004</v>
       </c>
       <c r="G5">
-        <v>0.15820000000000001</v>
+        <v>0.19117356776814501</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1848,16 +1855,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D6">
-        <v>-0.2359</v>
+        <v>-0.240490563657657</v>
       </c>
       <c r="E6">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.2979244410996999E-2</v>
       </c>
       <c r="F6">
         <v>0.80410000000000004</v>
       </c>
       <c r="G6">
-        <v>0.15820000000000001</v>
+        <v>0.16200582133621699</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1871,16 +1878,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-0.2359</v>
+        <v>-0.240490563657657</v>
       </c>
       <c r="E7">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.2979244410996999E-2</v>
       </c>
       <c r="F7">
         <v>0.80410000000000004</v>
       </c>
       <c r="G7">
-        <v>0.15820000000000001</v>
+        <v>0.16200582133621699</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1894,16 +1901,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D8">
-        <v>-0.2359</v>
+        <v>-9.9407806758646203E-2</v>
       </c>
       <c r="E8">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.2078264147537801E-2</v>
       </c>
       <c r="F8">
         <v>0.80410000000000004</v>
       </c>
       <c r="G8">
-        <v>0.15820000000000001</v>
+        <v>0.136668886034159</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1917,16 +1924,16 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-0.2359</v>
+        <v>-9.9407806758646203E-2</v>
       </c>
       <c r="E9">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.2078264147537801E-2</v>
       </c>
       <c r="F9">
         <v>0.80410000000000004</v>
       </c>
       <c r="G9">
-        <v>0.15820000000000001</v>
+        <v>0.136668886034159</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1940,16 +1947,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D10">
-        <v>-0.2359</v>
+        <v>-0.27797349965302398</v>
       </c>
       <c r="E10">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.3735710699773103E-2</v>
       </c>
       <c r="F10">
         <v>0.80410000000000004</v>
       </c>
       <c r="G10">
-        <v>0.15820000000000001</v>
+        <v>0.106997365635085</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1963,16 +1970,16 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>-0.2359</v>
+        <v>-0.27797349965302398</v>
       </c>
       <c r="E11">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.3735710699773103E-2</v>
       </c>
       <c r="F11">
         <v>0.80410000000000004</v>
       </c>
       <c r="G11">
-        <v>0.15820000000000001</v>
+        <v>0.106997365635085</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1986,16 +1993,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D12">
-        <v>-0.2359</v>
+        <v>-0.142376022666719</v>
       </c>
       <c r="E12">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4358816265883106E-2</v>
       </c>
       <c r="F12">
         <v>0.80410000000000004</v>
       </c>
       <c r="G12">
-        <v>0.15820000000000001</v>
+        <v>0.234706653372145</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2009,16 +2016,16 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>-0.2359</v>
+        <v>-0.142376022666719</v>
       </c>
       <c r="E13">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4358816265883106E-2</v>
       </c>
       <c r="F13">
         <v>0.80410000000000004</v>
       </c>
       <c r="G13">
-        <v>0.15820000000000001</v>
+        <v>0.234706653372145</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2032,16 +2039,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D14">
-        <v>-0.2359</v>
+        <v>-0.208086806776278</v>
       </c>
       <c r="E14">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6486252438383197E-2</v>
       </c>
       <c r="F14">
         <v>0.80410000000000004</v>
       </c>
       <c r="G14">
-        <v>0.15820000000000001</v>
+        <v>0.18449635759480501</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2055,16 +2062,16 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>-0.2359</v>
+        <v>-0.208086806776278</v>
       </c>
       <c r="E15">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6486252438383197E-2</v>
       </c>
       <c r="F15">
         <v>0.80410000000000004</v>
       </c>
       <c r="G15">
-        <v>0.15820000000000001</v>
+        <v>0.18449635759480501</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2078,16 +2085,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D16">
-        <v>-0.2359</v>
+        <v>-1.50967534831115E-2</v>
       </c>
       <c r="E16">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.4015859146499299E-2</v>
       </c>
       <c r="F16">
         <v>0.80410000000000004</v>
       </c>
       <c r="G16">
-        <v>0.15820000000000001</v>
+        <v>0.15690002641624901</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2101,16 +2108,16 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>-0.2359</v>
+        <v>-1.50967534831115E-2</v>
       </c>
       <c r="E17">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.4015859146499299E-2</v>
       </c>
       <c r="F17">
         <v>0.80410000000000004</v>
       </c>
       <c r="G17">
-        <v>0.15820000000000001</v>
+        <v>0.15690002641624901</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2124,16 +2131,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D18">
-        <v>-0.2359</v>
+        <v>-0.35421099601364903</v>
       </c>
       <c r="E18">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.2664335694490207E-2</v>
       </c>
       <c r="F18">
         <v>0.80410000000000004</v>
       </c>
       <c r="G18">
-        <v>0.15820000000000001</v>
+        <v>0.13139107817918899</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2147,16 +2154,16 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>-0.2359</v>
+        <v>-0.35421099601364903</v>
       </c>
       <c r="E19">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.2664335694490207E-2</v>
       </c>
       <c r="F19">
         <v>0.80410000000000004</v>
       </c>
       <c r="G19">
-        <v>0.15820000000000001</v>
+        <v>0.13139107817918899</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2170,16 +2177,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D20">
-        <v>-0.2359</v>
+        <v>-0.184516719067046</v>
       </c>
       <c r="E20">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5871306440246397E-2</v>
       </c>
       <c r="F20">
         <v>0.80410000000000004</v>
       </c>
       <c r="G20">
-        <v>0.15820000000000001</v>
+        <v>9.92137122552217E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2193,16 +2200,16 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>-0.2359</v>
+        <v>-0.184516719067046</v>
       </c>
       <c r="E21">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5871306440246397E-2</v>
       </c>
       <c r="F21">
         <v>0.80410000000000004</v>
       </c>
       <c r="G21">
-        <v>0.15820000000000001</v>
+        <v>9.92137122552217E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2216,16 +2223,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D22">
-        <v>-0.2359</v>
+        <v>-0.249153673764685</v>
       </c>
       <c r="E22">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8468993238358701E-2</v>
       </c>
       <c r="F22">
         <v>0.80410000000000004</v>
       </c>
       <c r="G22">
-        <v>0.15820000000000001</v>
+        <v>0.21857165259960801</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2239,16 +2246,16 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>-0.2359</v>
+        <v>-0.249153673764685</v>
       </c>
       <c r="E23">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8468993238358701E-2</v>
       </c>
       <c r="F23">
         <v>0.80410000000000004</v>
       </c>
       <c r="G23">
-        <v>0.15820000000000001</v>
+        <v>0.21857165259960801</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2262,16 +2269,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D24">
-        <v>-0.2359</v>
+        <v>-0.11164758217559</v>
       </c>
       <c r="E24">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.9699122074242698E-2</v>
       </c>
       <c r="F24">
         <v>0.80410000000000004</v>
       </c>
       <c r="G24">
-        <v>0.15820000000000001</v>
+        <v>0.17838490366929899</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2285,16 +2292,16 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>-0.2359</v>
+        <v>-0.11164758217559</v>
       </c>
       <c r="E25">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.9699122074242698E-2</v>
       </c>
       <c r="F25">
         <v>0.80410000000000004</v>
       </c>
       <c r="G25">
-        <v>0.15820000000000001</v>
+        <v>0.17838490366929899</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2308,16 +2315,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D26">
-        <v>-0.2359</v>
+        <v>-0.28907806181916301</v>
       </c>
       <c r="E26">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.0217772648956299E-2</v>
       </c>
       <c r="F26">
         <v>0.80410000000000004</v>
       </c>
       <c r="G26">
-        <v>0.15820000000000001</v>
+        <v>0.15186536405861401</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2331,16 +2338,16 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>-0.2359</v>
+        <v>-0.28907806181916301</v>
       </c>
       <c r="E27">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.0217772648956299E-2</v>
       </c>
       <c r="F27">
         <v>0.80410000000000004</v>
       </c>
       <c r="G27">
-        <v>0.15820000000000001</v>
+        <v>0.15186536405861401</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2354,16 +2361,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D28">
-        <v>-0.2359</v>
+        <v>-0.15139801962434701</v>
       </c>
       <c r="E28">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0996409219999601E-2</v>
       </c>
       <c r="F28">
         <v>0.80410000000000004</v>
       </c>
       <c r="G28">
-        <v>0.15820000000000001</v>
+        <v>0.125896766033716</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2377,16 +2384,16 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>-0.2359</v>
+        <v>-0.15139801962434701</v>
       </c>
       <c r="E29">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0996409219999601E-2</v>
       </c>
       <c r="F29">
         <v>0.80410000000000004</v>
       </c>
       <c r="G29">
-        <v>0.15820000000000001</v>
+        <v>0.125896766033716</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2400,16 +2407,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D30">
-        <v>-0.2359</v>
+        <v>-0.215978952613544</v>
       </c>
       <c r="E30">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.20492037846051E-2</v>
       </c>
       <c r="F30">
         <v>0.80410000000000004</v>
       </c>
       <c r="G30">
-        <v>0.15820000000000001</v>
+        <v>8.9951134108337202E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2423,16 +2430,16 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>-0.2359</v>
+        <v>-0.215978952613544</v>
       </c>
       <c r="E31">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.20492037846051E-2</v>
       </c>
       <c r="F31">
         <v>0.80410000000000004</v>
       </c>
       <c r="G31">
-        <v>0.15820000000000001</v>
+        <v>8.9951134108337202E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2446,16 +2453,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D32">
-        <v>-0.2359</v>
+        <v>-4.7377213035161403E-2</v>
       </c>
       <c r="E32">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.4581935844978701E-2</v>
       </c>
       <c r="F32">
         <v>0.80410000000000004</v>
       </c>
       <c r="G32">
-        <v>0.15820000000000001</v>
+        <v>0.207488331847902</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2469,16 +2476,16 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>-0.2359</v>
+        <v>-4.7377213035161403E-2</v>
       </c>
       <c r="E33">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.4581935844978701E-2</v>
       </c>
       <c r="F33">
         <v>0.80410000000000004</v>
       </c>
       <c r="G33">
-        <v>0.15820000000000001</v>
+        <v>0.207488331847902</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2492,16 +2499,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D34">
-        <v>-0.2359</v>
+        <v>-0.31551063577765598</v>
       </c>
       <c r="E34">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.8887627835544499E-2</v>
       </c>
       <c r="F34">
         <v>0.80410000000000004</v>
       </c>
       <c r="G34">
-        <v>0.15820000000000001</v>
+        <v>0.17267144014616601</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2515,16 +2522,16 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>-0.2359</v>
+        <v>-0.31551063577765598</v>
       </c>
       <c r="E35">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.8887627835544499E-2</v>
       </c>
       <c r="F35">
         <v>0.80410000000000004</v>
       </c>
       <c r="G35">
-        <v>0.15820000000000001</v>
+        <v>0.17267144014616601</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2538,16 +2545,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D36">
-        <v>-0.2359</v>
+        <v>-0.16839349381360599</v>
       </c>
       <c r="E36">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.7032363994672406E-2</v>
       </c>
       <c r="F36">
         <v>0.80410000000000004</v>
       </c>
       <c r="G36">
-        <v>0.15820000000000001</v>
+        <v>0.14684959159223601</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2561,16 +2568,16 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>-0.2359</v>
+        <v>-0.16839349381360599</v>
       </c>
       <c r="E37">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.7032363994672406E-2</v>
       </c>
       <c r="F37">
         <v>0.80410000000000004</v>
       </c>
       <c r="G37">
-        <v>0.15820000000000001</v>
+        <v>0.14684959159223601</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2584,16 +2591,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D38">
-        <v>-0.2359</v>
+        <v>-0.232121577943501</v>
       </c>
       <c r="E38">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3956955859383898E-2</v>
       </c>
       <c r="F38">
         <v>0.80410000000000004</v>
       </c>
       <c r="G38">
-        <v>0.15820000000000001</v>
+        <v>0.12009401002820801</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2607,16 +2614,16 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>-0.2359</v>
+        <v>-0.232121577943501</v>
       </c>
       <c r="E39">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3956955859383898E-2</v>
       </c>
       <c r="F39">
         <v>0.80410000000000004</v>
       </c>
       <c r="G39">
-        <v>0.15820000000000001</v>
+        <v>0.12009401002820801</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2630,16 +2637,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D40">
-        <v>-0.2359</v>
+        <v>-8.5438170742219405E-2</v>
       </c>
       <c r="E40">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.6199204718611898E-2</v>
       </c>
       <c r="F40">
         <v>0.80410000000000004</v>
       </c>
       <c r="G40">
-        <v>0.15820000000000001</v>
+        <v>7.7981014339295607E-2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2653,16 +2660,16 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>-0.2359</v>
+        <v>-8.5438170742219405E-2</v>
       </c>
       <c r="E41">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.6199204718611898E-2</v>
       </c>
       <c r="F41">
         <v>0.80410000000000004</v>
       </c>
       <c r="G41">
-        <v>0.15820000000000001</v>
+        <v>7.7981014339295607E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2676,16 +2683,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D42">
-        <v>-0.2359</v>
+        <v>-0.267756605483219</v>
       </c>
       <c r="E42">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.6878199726893198E-2</v>
       </c>
       <c r="F42">
         <v>0.80410000000000004</v>
       </c>
       <c r="G42">
-        <v>0.15820000000000001</v>
+        <v>0.19868152870184899</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2699,16 +2706,16 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>-0.2359</v>
+        <v>-0.267756605483219</v>
       </c>
       <c r="E43">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.6878199726893198E-2</v>
       </c>
       <c r="F43">
         <v>0.80410000000000004</v>
       </c>
       <c r="G43">
-        <v>0.15820000000000001</v>
+        <v>0.19868152870184899</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2722,16 +2729,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D44">
-        <v>-0.2359</v>
+        <v>-0.13285801845048401</v>
       </c>
       <c r="E44">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.83591678252435E-2</v>
       </c>
       <c r="F44">
         <v>0.80410000000000004</v>
       </c>
       <c r="G44">
-        <v>0.15820000000000001</v>
+        <v>0.16724031476746901</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2745,16 +2752,16 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>-0.2359</v>
+        <v>-0.13285801845048401</v>
       </c>
       <c r="E45">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.83591678252435E-2</v>
       </c>
       <c r="F45">
         <v>0.80410000000000004</v>
       </c>
       <c r="G45">
-        <v>0.15820000000000001</v>
+        <v>0.16724031476746901</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2768,16 +2775,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D46">
-        <v>-0.2359</v>
+        <v>-0.20024478816191099</v>
       </c>
       <c r="E46">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.78439425514901E-2</v>
       </c>
       <c r="F46">
         <v>0.80410000000000004</v>
       </c>
       <c r="G46">
-        <v>0.15820000000000001</v>
+        <v>0.14180183277015301</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2791,16 +2798,16 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>-0.2359</v>
+        <v>-0.20024478816191099</v>
       </c>
       <c r="E47">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.78439425514901E-2</v>
       </c>
       <c r="F47">
         <v>0.80410000000000004</v>
       </c>
       <c r="G47">
-        <v>0.15820000000000001</v>
+        <v>0.14180183277015301</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2813,17 +2820,17 @@
       <c r="C48">
         <v>-0.3422</v>
       </c>
-      <c r="D48">
-        <v>-0.2359</v>
+      <c r="D48" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E48">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.9890316597160403E-2</v>
       </c>
       <c r="F48">
         <v>0.80410000000000004</v>
       </c>
       <c r="G48">
-        <v>0.15820000000000001</v>
+        <v>0.113856519837811</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2836,17 +2843,17 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49">
-        <v>-0.2359</v>
+      <c r="D49" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E49">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.9890316597160403E-2</v>
       </c>
       <c r="F49">
         <v>0.80410000000000004</v>
       </c>
       <c r="G49">
-        <v>0.15820000000000001</v>
+        <v>0.113856519837811</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2860,16 +2867,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D50">
-        <v>-0.2359</v>
+        <v>-0.52971933456919595</v>
       </c>
       <c r="E50">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.2627074635817698E-2</v>
       </c>
       <c r="F50">
         <v>0.80410000000000004</v>
       </c>
       <c r="G50">
-        <v>0.15820000000000001</v>
+        <v>5.9326707131112301E-2</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2883,16 +2890,16 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>-0.2359</v>
+        <v>-0.52971933456919595</v>
       </c>
       <c r="E51">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.2627074635817698E-2</v>
       </c>
       <c r="F51">
         <v>0.80410000000000004</v>
       </c>
       <c r="G51">
-        <v>0.15820000000000001</v>
+        <v>5.9326707131112301E-2</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2906,16 +2913,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D52">
-        <v>-0.2359</v>
+        <v>-0.19987760601071899</v>
       </c>
       <c r="E52">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.00414899038063E-2</v>
       </c>
       <c r="F52">
         <v>0.80410000000000004</v>
       </c>
       <c r="G52">
-        <v>0.15820000000000001</v>
+        <v>0.26113206276743001</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2929,16 +2936,16 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>-0.2359</v>
+        <v>-0.19987760601071899</v>
       </c>
       <c r="E53">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.00414899038063E-2</v>
       </c>
       <c r="F53">
         <v>0.80410000000000004</v>
       </c>
       <c r="G53">
-        <v>0.15820000000000001</v>
+        <v>0.26113206276743001</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2952,16 +2959,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D54">
-        <v>-0.2359</v>
+        <v>-0.26729539900635102</v>
       </c>
       <c r="E54">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.8691789107803204E-2</v>
       </c>
       <c r="F54">
         <v>0.80410000000000004</v>
       </c>
       <c r="G54">
-        <v>0.15820000000000001</v>
+        <v>0.18978211267133499</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2975,16 +2982,16 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>-0.2359</v>
+        <v>-0.26729539900635102</v>
       </c>
       <c r="E55">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.8691789107803204E-2</v>
       </c>
       <c r="F55">
         <v>0.80410000000000004</v>
       </c>
       <c r="G55">
-        <v>0.15820000000000001</v>
+        <v>0.18978211267133499</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2998,16 +3005,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D56">
-        <v>-0.2359</v>
+        <v>-0.13239728971966899</v>
       </c>
       <c r="E56">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7176998506343099E-2</v>
       </c>
       <c r="F56">
         <v>0.80410000000000004</v>
       </c>
       <c r="G56">
-        <v>0.15820000000000001</v>
+        <v>0.160976321100675</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -3021,16 +3028,16 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>-0.2359</v>
+        <v>-0.13239728971966899</v>
       </c>
       <c r="E57">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7176998506343099E-2</v>
       </c>
       <c r="F57">
         <v>0.80410000000000004</v>
       </c>
       <c r="G57">
-        <v>0.15820000000000001</v>
+        <v>0.160976321100675</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -3044,16 +3051,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D58">
-        <v>-0.2359</v>
+        <v>-0.31479806245425501</v>
       </c>
       <c r="E58">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.9901911660536499E-2</v>
       </c>
       <c r="F58">
         <v>0.80410000000000004</v>
       </c>
       <c r="G58">
-        <v>0.15820000000000001</v>
+        <v>0.135626991811719</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -3067,16 +3074,16 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>-0.2359</v>
+        <v>-0.31479806245425501</v>
       </c>
       <c r="E59">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.9901911660536499E-2</v>
       </c>
       <c r="F59">
         <v>0.80410000000000004</v>
       </c>
       <c r="G59">
-        <v>0.15820000000000001</v>
+        <v>0.135626991811719</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -3090,16 +3097,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D60">
-        <v>-0.2359</v>
+        <v>-0.16800726937567501</v>
       </c>
       <c r="E60">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.1820452954081099E-2</v>
       </c>
       <c r="F60">
         <v>0.80410000000000004</v>
       </c>
       <c r="G60">
-        <v>0.15820000000000001</v>
+        <v>0.10552738054232</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -3113,16 +3120,16 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>-0.2359</v>
+        <v>-0.16800726937567501</v>
       </c>
       <c r="E61">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.1820452954081099E-2</v>
       </c>
       <c r="F61">
         <v>0.80410000000000004</v>
       </c>
       <c r="G61">
-        <v>0.15820000000000001</v>
+        <v>0.10552738054232</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -3136,16 +3143,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D62">
-        <v>-0.2359</v>
+        <v>-0.23173519500263901</v>
       </c>
       <c r="E62">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.1456896916844998E-2</v>
       </c>
       <c r="F62">
         <v>0.80410000000000004</v>
       </c>
       <c r="G62">
-        <v>0.15820000000000001</v>
+        <v>0.23076632680604101</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -3159,16 +3166,16 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>-0.2359</v>
+        <v>-0.23173519500263901</v>
       </c>
       <c r="E63">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.1456896916844998E-2</v>
       </c>
       <c r="F63">
         <v>0.80410000000000004</v>
       </c>
       <c r="G63">
-        <v>0.15820000000000001</v>
+        <v>0.23076632680604101</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -3182,16 +3189,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D64">
-        <v>-0.2359</v>
+        <v>-8.4727539152596301E-2</v>
       </c>
       <c r="E64">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.2858511321528998E-2</v>
       </c>
       <c r="F64">
         <v>0.80410000000000004</v>
       </c>
       <c r="G64">
-        <v>0.15820000000000001</v>
+        <v>0.18323518709658501</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -3205,16 +3212,16 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>-0.2359</v>
+        <v>-8.4727539152596301E-2</v>
       </c>
       <c r="E65">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.2858511321528998E-2</v>
       </c>
       <c r="F65">
         <v>0.80410000000000004</v>
       </c>
       <c r="G65">
-        <v>0.15820000000000001</v>
+        <v>0.18323518709658501</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -3228,16 +3235,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D66">
-        <v>-0.2359</v>
+        <v>-0.35301622919752002</v>
       </c>
       <c r="E66">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.3569040276474406E-2</v>
       </c>
       <c r="F66">
         <v>0.80410000000000004</v>
       </c>
       <c r="G66">
-        <v>0.15820000000000001</v>
+        <v>0.15588912474738201</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -3251,16 +3258,16 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>-0.2359</v>
+        <v>-0.35301622919752002</v>
       </c>
       <c r="E67">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.3569040276474406E-2</v>
       </c>
       <c r="F67">
         <v>0.80410000000000004</v>
       </c>
       <c r="G67">
-        <v>0.15820000000000001</v>
+        <v>0.15588912474738201</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -3274,16 +3281,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D68">
-        <v>-0.2359</v>
+        <v>-0.184145001640661</v>
       </c>
       <c r="E68">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.5855859824167899E-2</v>
       </c>
       <c r="F68">
         <v>0.80410000000000004</v>
       </c>
       <c r="G68">
-        <v>0.15820000000000001</v>
+        <v>0.130312119260098</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3297,16 +3304,16 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>-0.2359</v>
+        <v>-0.184145001640661</v>
       </c>
       <c r="E69">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.5855859824167899E-2</v>
       </c>
       <c r="F69">
         <v>0.80410000000000004</v>
       </c>
       <c r="G69">
-        <v>0.15820000000000001</v>
+        <v>0.130312119260098</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3320,16 +3327,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D70">
-        <v>-0.2359</v>
+        <v>-0.24873976444756299</v>
       </c>
       <c r="E70">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.25032305148378E-2</v>
       </c>
       <c r="F70">
         <v>0.80410000000000004</v>
       </c>
       <c r="G70">
-        <v>0.15820000000000001</v>
+        <v>9.7504555078177901E-2</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3343,16 +3350,16 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>-0.2359</v>
+        <v>-0.24873976444756299</v>
       </c>
       <c r="E71">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.25032305148378E-2</v>
       </c>
       <c r="F71">
         <v>0.80410000000000004</v>
       </c>
       <c r="G71">
-        <v>0.15820000000000001</v>
+        <v>9.7504555078177901E-2</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3366,16 +3373,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D72">
-        <v>-0.2359</v>
+        <v>-0.11110378788924299</v>
       </c>
       <c r="E72">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.0511578092186994E-2</v>
       </c>
       <c r="F72">
         <v>0.80410000000000004</v>
       </c>
       <c r="G72">
-        <v>0.15820000000000001</v>
+        <v>0.21608921316579399</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3389,16 +3396,16 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>-0.2359</v>
+        <v>-0.11110378788924299</v>
       </c>
       <c r="E73">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.0511578092186994E-2</v>
       </c>
       <c r="F73">
         <v>0.80410000000000004</v>
       </c>
       <c r="G73">
-        <v>0.15820000000000001</v>
+        <v>0.21608921316579399</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3412,16 +3419,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D74">
-        <v>-0.2359</v>
+        <v>-0.28853339165015202</v>
       </c>
       <c r="E74">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5228067989375101E-2</v>
       </c>
       <c r="F74">
         <v>0.80410000000000004</v>
       </c>
       <c r="G74">
-        <v>0.15820000000000001</v>
+        <v>0.17721464005632301</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3435,16 +3442,16 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>-0.2359</v>
+        <v>-0.28853339165015202</v>
       </c>
       <c r="E75">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5228067989375101E-2</v>
       </c>
       <c r="F75">
         <v>0.80410000000000004</v>
       </c>
       <c r="G75">
-        <v>0.15820000000000001</v>
+        <v>0.17721464005632301</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3458,16 +3465,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D76">
-        <v>-0.2359</v>
+        <v>-0.150984389245651</v>
       </c>
       <c r="E76">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.7730185012748198E-2</v>
       </c>
       <c r="F76">
         <v>0.80410000000000004</v>
       </c>
       <c r="G76">
-        <v>0.15820000000000001</v>
+        <v>0.150862322872827</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3481,16 +3488,16 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>-0.2359</v>
+        <v>-0.150984389245651</v>
       </c>
       <c r="E77">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.7730185012748198E-2</v>
       </c>
       <c r="F77">
         <v>0.80410000000000004</v>
       </c>
       <c r="G77">
-        <v>0.15820000000000001</v>
+        <v>0.150862322872827</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3504,16 +3511,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D78">
-        <v>-0.2359</v>
+        <v>-0.215607162718745</v>
       </c>
       <c r="E78">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.8717521712099994E-2</v>
       </c>
       <c r="F78">
         <v>0.80410000000000004</v>
       </c>
       <c r="G78">
-        <v>0.15820000000000001</v>
+        <v>0.124764319466211</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3527,16 +3534,16 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>-0.2359</v>
+        <v>-0.215607162718745</v>
       </c>
       <c r="E79">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.8717521712099994E-2</v>
       </c>
       <c r="F79">
         <v>0.80410000000000004</v>
       </c>
       <c r="G79">
-        <v>0.15820000000000001</v>
+        <v>0.124764319466211</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3550,16 +3557,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D80">
-        <v>-0.2359</v>
+        <v>-4.6189702001336902E-2</v>
       </c>
       <c r="E80">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.9598820882561602E-2</v>
       </c>
       <c r="F80">
         <v>0.80410000000000004</v>
       </c>
       <c r="G80">
-        <v>0.15820000000000001</v>
+        <v>8.78353659127772E-2</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3573,16 +3580,16 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>-0.2359</v>
+        <v>-4.6189702001336902E-2</v>
       </c>
       <c r="E81">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.9598820882561602E-2</v>
       </c>
       <c r="F81">
         <v>0.80410000000000004</v>
       </c>
       <c r="G81">
-        <v>0.15820000000000001</v>
+        <v>8.78353659127772E-2</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3596,16 +3603,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D82">
-        <v>-0.2359</v>
+        <v>-0.38558386304624198</v>
       </c>
       <c r="E82">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0000792125242499E-2</v>
       </c>
       <c r="F82">
         <v>0.80410000000000004</v>
       </c>
       <c r="G82">
-        <v>0.15820000000000001</v>
+        <v>0.20558815747089501</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3619,16 +3626,16 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>-0.2359</v>
+        <v>-0.38558386304624198</v>
       </c>
       <c r="E83">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0000792125242499E-2</v>
       </c>
       <c r="F83">
         <v>0.80410000000000004</v>
       </c>
       <c r="G83">
-        <v>0.15820000000000001</v>
+        <v>0.20558815747089501</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3642,16 +3649,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D84">
-        <v>-0.2359</v>
+        <v>-0.192035981978326</v>
       </c>
       <c r="E84">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.1315133164767603E-2</v>
       </c>
       <c r="F84">
         <v>0.80410000000000004</v>
       </c>
       <c r="G84">
-        <v>0.15820000000000001</v>
+        <v>0.17156570495913601</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3665,16 +3672,16 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>-0.2359</v>
+        <v>-0.192035981978326</v>
       </c>
       <c r="E85">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.1315133164767603E-2</v>
       </c>
       <c r="F85">
         <v>0.80410000000000004</v>
       </c>
       <c r="G85">
-        <v>0.15820000000000001</v>
+        <v>0.17156570495913601</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3688,16 +3695,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D86">
-        <v>-0.2359</v>
+        <v>-0.25776853636857</v>
       </c>
       <c r="E86">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.3936962430468199E-2</v>
       </c>
       <c r="F86">
         <v>0.80410000000000004</v>
       </c>
       <c r="G86">
-        <v>0.15820000000000001</v>
+        <v>0.145844243784715</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3711,16 +3718,16 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>-0.2359</v>
+        <v>-0.25776853636857</v>
       </c>
       <c r="E87">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.3936962430468199E-2</v>
       </c>
       <c r="F87">
         <v>0.80410000000000004</v>
       </c>
       <c r="G87">
-        <v>0.15820000000000001</v>
+        <v>0.145844243784715</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3734,16 +3741,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D88">
-        <v>-0.2359</v>
+        <v>-0.12219226888321</v>
       </c>
       <c r="E88">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.66189981816444E-2</v>
       </c>
       <c r="F88">
         <v>0.80410000000000004</v>
       </c>
       <c r="G88">
-        <v>0.15820000000000001</v>
+        <v>0.118886169610286</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3757,16 +3764,16 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>-0.2359</v>
+        <v>-0.12219226888321</v>
       </c>
       <c r="E89">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.66189981816444E-2</v>
       </c>
       <c r="F89">
         <v>0.80410000000000004</v>
       </c>
       <c r="G89">
-        <v>0.15820000000000001</v>
+        <v>0.118886169610286</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3780,16 +3787,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D90">
-        <v>-0.2359</v>
+        <v>-0.300795396555668</v>
       </c>
       <c r="E90">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.5563436784146704E-2</v>
       </c>
       <c r="F90">
         <v>0.80410000000000004</v>
       </c>
       <c r="G90">
-        <v>0.15820000000000001</v>
+        <v>7.5028091960408702E-2</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3803,16 +3810,16 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>-0.2359</v>
+        <v>-0.300795396555668</v>
       </c>
       <c r="E91">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.5563436784146704E-2</v>
       </c>
       <c r="F91">
         <v>0.80410000000000004</v>
       </c>
       <c r="G91">
-        <v>0.15820000000000001</v>
+        <v>7.5028091960408702E-2</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3826,16 +3833,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D92">
-        <v>-0.2359</v>
+        <v>-0.15964225048075101</v>
       </c>
       <c r="E92">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3327661059490501E-2</v>
       </c>
       <c r="F92">
         <v>0.80410000000000004</v>
       </c>
       <c r="G92">
-        <v>0.15820000000000001</v>
+        <v>0.19709537499527699</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3849,16 +3856,16 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>-0.2359</v>
+        <v>-0.15964225048075101</v>
       </c>
       <c r="E93">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3327661059490501E-2</v>
       </c>
       <c r="F93">
         <v>0.80410000000000004</v>
       </c>
       <c r="G93">
-        <v>0.15820000000000001</v>
+        <v>0.19709537499527699</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3872,16 +3879,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D94">
-        <v>-0.2359</v>
+        <v>-0.223594343603256</v>
       </c>
       <c r="E94">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.54028673578397E-2</v>
       </c>
       <c r="F94">
         <v>0.80410000000000004</v>
       </c>
       <c r="G94">
-        <v>0.15820000000000001</v>
+        <v>0.16618005863617699</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3895,16 +3902,16 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <v>-0.2359</v>
+        <v>-0.223594343603256</v>
       </c>
       <c r="E95">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.54028673578397E-2</v>
       </c>
       <c r="F95">
         <v>0.80410000000000004</v>
       </c>
       <c r="G95">
-        <v>0.15820000000000001</v>
+        <v>0.16618005863617699</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3918,16 +3925,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D96">
-        <v>-0.2359</v>
+        <v>-6.7906619705671897E-2</v>
       </c>
       <c r="E96">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.6010348725465198E-2</v>
       </c>
       <c r="F96">
         <v>0.80410000000000004</v>
       </c>
       <c r="G96">
-        <v>0.15820000000000001</v>
+        <v>0.140783845432841</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3941,16 +3948,16 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <v>-0.2359</v>
+        <v>-6.7906619705671897E-2</v>
       </c>
       <c r="E97">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.6010348725465198E-2</v>
       </c>
       <c r="F97">
         <v>0.80410000000000004</v>
       </c>
       <c r="G97">
-        <v>0.15820000000000001</v>
+        <v>0.140783845432841</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3964,16 +3971,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D98">
-        <v>-0.2359</v>
+        <v>-0.33150992087530001</v>
       </c>
       <c r="E98">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.7737268234379203E-2</v>
       </c>
       <c r="F98">
         <v>0.80410000000000004</v>
       </c>
       <c r="G98">
-        <v>0.15820000000000001</v>
+        <v>0.112541935703094</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3987,16 +3994,16 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <v>-0.2359</v>
+        <v>-0.33150992087530001</v>
       </c>
       <c r="E99">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.7737268234379203E-2</v>
       </c>
       <c r="F99">
         <v>0.80410000000000004</v>
       </c>
       <c r="G99">
-        <v>0.15820000000000001</v>
+        <v>0.112541935703094</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -4010,16 +4017,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D100">
-        <v>-0.2359</v>
+        <v>-0.176153884147315</v>
       </c>
       <c r="E100">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.66622399342267E-2</v>
       </c>
       <c r="F100">
         <v>0.80410000000000004</v>
       </c>
       <c r="G100">
-        <v>0.15820000000000001</v>
+        <v>5.3561732803062201E-2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -4033,16 +4040,16 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <v>-0.2359</v>
+        <v>-0.176153884147315</v>
       </c>
       <c r="E101">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.66622399342267E-2</v>
       </c>
       <c r="F101">
         <v>0.80410000000000004</v>
       </c>
       <c r="G101">
-        <v>0.15820000000000001</v>
+        <v>5.3561732803062201E-2</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -4056,16 +4063,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D102">
-        <v>-0.2359</v>
+        <v>-0.24009233438658201</v>
       </c>
       <c r="E102">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.9196738203285602E-2</v>
       </c>
       <c r="F102">
         <v>0.80410000000000004</v>
       </c>
       <c r="G102">
-        <v>0.15820000000000001</v>
+        <v>0.25155739186431397</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -4079,16 +4086,16 @@
         <v>0</v>
       </c>
       <c r="D103">
-        <v>-0.2359</v>
+        <v>-0.24009233438658201</v>
       </c>
       <c r="E103">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.9196738203285602E-2</v>
       </c>
       <c r="F103">
         <v>0.80410000000000004</v>
       </c>
       <c r="G103">
-        <v>0.15820000000000001</v>
+        <v>0.25155739186431397</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4102,16 +4109,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D104">
-        <v>-0.2359</v>
+        <v>-9.8796943087606198E-2</v>
       </c>
       <c r="E104">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.19604353389227E-2</v>
       </c>
       <c r="F104">
         <v>0.80410000000000004</v>
       </c>
       <c r="G104">
-        <v>0.15820000000000001</v>
+        <v>0.188420806543214</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -4125,16 +4132,16 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <v>-0.2359</v>
+        <v>-9.8796943087606198E-2</v>
       </c>
       <c r="E105">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.19604353389227E-2</v>
       </c>
       <c r="F105">
         <v>0.80410000000000004</v>
       </c>
       <c r="G105">
-        <v>0.15820000000000001</v>
+        <v>0.188420806543214</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -4148,16 +4155,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D106">
-        <v>-0.2359</v>
+        <v>-0.27747683364501802</v>
       </c>
       <c r="E106">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.85230443661253E-3</v>
       </c>
       <c r="F106">
         <v>0.80410000000000004</v>
       </c>
       <c r="G106">
-        <v>0.15820000000000001</v>
+        <v>0.159951453813239</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -4171,16 +4178,16 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <v>-0.2359</v>
+        <v>-0.27747683364501802</v>
       </c>
       <c r="E107">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.85230443661253E-3</v>
       </c>
       <c r="F107">
         <v>0.80410000000000004</v>
       </c>
       <c r="G107">
-        <v>0.15820000000000001</v>
+        <v>0.159951453813239</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -4194,16 +4201,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D108">
-        <v>-0.2359</v>
+        <v>-0.14194198259027299</v>
       </c>
       <c r="E108">
-        <v>-4.8800000000000003E-2</v>
+        <v>-0.100308775949178</v>
       </c>
       <c r="F108">
         <v>0.80410000000000004</v>
       </c>
       <c r="G108">
-        <v>0.15820000000000001</v>
+        <v>0.13457881826043799</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -4217,16 +4224,16 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <v>-0.2359</v>
+        <v>-0.14194198259027299</v>
       </c>
       <c r="E109">
-        <v>-4.8800000000000003E-2</v>
+        <v>-0.100308775949178</v>
       </c>
       <c r="F109">
         <v>0.80410000000000004</v>
       </c>
       <c r="G109">
-        <v>0.15820000000000001</v>
+        <v>0.13457881826043799</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -4240,16 +4247,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D110">
-        <v>-0.2359</v>
+        <v>-0.207718476343804</v>
       </c>
       <c r="E110">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.8288712635946399E-2</v>
       </c>
       <c r="F110">
         <v>0.80410000000000004</v>
       </c>
       <c r="G110">
-        <v>0.15820000000000001</v>
+        <v>0.104017912336008</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -4263,16 +4270,16 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <v>-0.2359</v>
+        <v>-0.207718476343804</v>
       </c>
       <c r="E111">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.8288712635946399E-2</v>
       </c>
       <c r="F111">
         <v>0.80410000000000004</v>
       </c>
       <c r="G111">
-        <v>0.15820000000000001</v>
+        <v>0.104017912336008</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -4286,16 +4293,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D112">
-        <v>-0.2359</v>
+        <v>-1.3028523107612201E-2</v>
       </c>
       <c r="E112">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.10573178822322E-2</v>
       </c>
       <c r="F112">
         <v>0.80410000000000004</v>
       </c>
       <c r="G112">
-        <v>0.15820000000000001</v>
+        <v>0.22727197337928801</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -4309,16 +4316,16 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <v>-0.2359</v>
+        <v>-1.3028523107612201E-2</v>
       </c>
       <c r="E113">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.10573178822322E-2</v>
       </c>
       <c r="F113">
         <v>0.80410000000000004</v>
       </c>
       <c r="G113">
-        <v>0.15820000000000001</v>
+        <v>0.22727197337928801</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -4332,16 +4339,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D114">
-        <v>-0.2359</v>
+        <v>-0.414158908914732</v>
       </c>
       <c r="E114">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.3796730337675698E-2</v>
       </c>
       <c r="F114">
         <v>0.80410000000000004</v>
       </c>
       <c r="G114">
-        <v>0.15820000000000001</v>
+        <v>0.181994816502413</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -4355,16 +4362,16 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <v>-0.2359</v>
+        <v>-0.414158908914732</v>
       </c>
       <c r="E115">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.3796730337675698E-2</v>
       </c>
       <c r="F115">
         <v>0.80410000000000004</v>
       </c>
       <c r="G115">
-        <v>0.15820000000000001</v>
+        <v>0.181994816502413</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -4378,16 +4385,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D116">
-        <v>-0.2359</v>
+        <v>-0.19595990056232099</v>
       </c>
       <c r="E116">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.2493589162442497E-2</v>
       </c>
       <c r="F116">
         <v>0.80410000000000004</v>
       </c>
       <c r="G116">
-        <v>0.15820000000000001</v>
+        <v>0.15488062489587201</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -4401,16 +4408,16 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <v>-0.2359</v>
+        <v>-0.19595990056232099</v>
       </c>
       <c r="E117">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.2493589162442497E-2</v>
       </c>
       <c r="F117">
         <v>0.80410000000000004</v>
       </c>
       <c r="G117">
-        <v>0.15820000000000001</v>
+        <v>0.15488062489587201</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -4424,16 +4431,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D118">
-        <v>-0.2359</v>
+        <v>-0.26246107499747401</v>
       </c>
       <c r="E118">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.4303494291412898E-2</v>
       </c>
       <c r="F118">
         <v>0.80410000000000004</v>
       </c>
       <c r="G118">
-        <v>0.15820000000000001</v>
+        <v>0.129223912745595</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -4447,16 +4454,16 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <v>-0.2359</v>
+        <v>-0.26246107499747401</v>
       </c>
       <c r="E119">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.4303494291412898E-2</v>
       </c>
       <c r="F119">
         <v>0.80410000000000004</v>
       </c>
       <c r="G119">
-        <v>0.15820000000000001</v>
+        <v>0.129223912745595</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4470,16 +4477,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D120">
-        <v>-0.2359</v>
+        <v>-0.12738934231714</v>
       </c>
       <c r="E120">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4897976812078706E-2</v>
       </c>
       <c r="F120">
         <v>0.80410000000000004</v>
       </c>
       <c r="G120">
-        <v>0.15820000000000001</v>
+        <v>9.5731746885326097E-2</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -4493,16 +4500,16 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <v>-0.2359</v>
+        <v>-0.12738934231714</v>
       </c>
       <c r="E121">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4897976812078706E-2</v>
       </c>
       <c r="F121">
         <v>0.80410000000000004</v>
       </c>
       <c r="G121">
-        <v>0.15820000000000001</v>
+        <v>9.5731746885326097E-2</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4516,16 +4523,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D122">
-        <v>-0.2359</v>
+        <v>-0.30753309985181698</v>
       </c>
       <c r="E122">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6904544558322402E-2</v>
       </c>
       <c r="F122">
         <v>0.80410000000000004</v>
       </c>
       <c r="G122">
-        <v>0.15820000000000001</v>
+        <v>0.21375978258533401</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4539,16 +4546,16 @@
         <v>0</v>
       </c>
       <c r="D123">
-        <v>-0.2359</v>
+        <v>-0.30753309985181698</v>
       </c>
       <c r="E123">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6904544558322402E-2</v>
       </c>
       <c r="F123">
         <v>0.80410000000000004</v>
       </c>
       <c r="G123">
-        <v>0.15820000000000001</v>
+        <v>0.21375978258533401</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -4562,16 +4569,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D124">
-        <v>-0.2359</v>
+        <v>-0.16385638625955701</v>
       </c>
       <c r="E124">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.49470373931216E-2</v>
       </c>
       <c r="F124">
         <v>0.80410000000000004</v>
       </c>
       <c r="G124">
-        <v>0.15820000000000001</v>
+        <v>0.176059099434002</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4585,16 +4592,16 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <v>-0.2359</v>
+        <v>-0.16385638625955701</v>
       </c>
       <c r="E125">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.49470373931216E-2</v>
       </c>
       <c r="F125">
         <v>0.80410000000000004</v>
       </c>
       <c r="G125">
-        <v>0.15820000000000001</v>
+        <v>0.176059099434002</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -4608,16 +4615,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D126">
-        <v>-0.2359</v>
+        <v>-0.22764186127654301</v>
       </c>
       <c r="E126">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.4341824449482197E-2</v>
       </c>
       <c r="F126">
         <v>0.80410000000000004</v>
       </c>
       <c r="G126">
-        <v>0.15820000000000001</v>
+        <v>0.14985962863222699</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -4631,16 +4638,16 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <v>-0.2359</v>
+        <v>-0.22764186127654301</v>
       </c>
       <c r="E127">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.4341824449482197E-2</v>
       </c>
       <c r="F127">
         <v>0.80410000000000004</v>
       </c>
       <c r="G127">
-        <v>0.15820000000000001</v>
+        <v>0.14985962863222699</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -4654,16 +4661,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D128">
-        <v>-0.2359</v>
+        <v>-7.6752965463390402E-2</v>
       </c>
       <c r="E128">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.6303489823695901E-2</v>
       </c>
       <c r="F128">
         <v>0.80410000000000004</v>
       </c>
       <c r="G128">
-        <v>0.15820000000000001</v>
+        <v>0.123618776092686</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4677,16 +4684,16 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <v>-0.2359</v>
+        <v>-7.6752965463390402E-2</v>
       </c>
       <c r="E129">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.6303489823695901E-2</v>
       </c>
       <c r="F129">
         <v>0.80410000000000004</v>
       </c>
       <c r="G129">
-        <v>0.15820000000000001</v>
+        <v>0.123618776092686</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -4700,16 +4707,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D130">
-        <v>-0.2359</v>
+        <v>-0.34144610955853799</v>
       </c>
       <c r="E130">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8952870972313897E-2</v>
       </c>
       <c r="F130">
         <v>0.80410000000000004</v>
       </c>
       <c r="G130">
-        <v>0.15820000000000001</v>
+        <v>8.5602016148145693E-2</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -4723,16 +4730,16 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <v>-0.2359</v>
+        <v>-0.34144610955853799</v>
       </c>
       <c r="E131">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8952870972313897E-2</v>
       </c>
       <c r="F131">
         <v>0.80410000000000004</v>
       </c>
       <c r="G131">
-        <v>0.15820000000000001</v>
+        <v>8.5602016148145693E-2</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -4746,16 +4753,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D132">
-        <v>-0.2359</v>
+        <v>-0.18016528160647199</v>
       </c>
       <c r="E132">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.0380768363822899E-2</v>
       </c>
       <c r="F132">
         <v>0.80410000000000004</v>
       </c>
       <c r="G132">
-        <v>0.15820000000000001</v>
+        <v>0.203765048732165</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -4769,16 +4776,16 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <v>-0.2359</v>
+        <v>-0.18016528160647199</v>
       </c>
       <c r="E133">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.0380768363822899E-2</v>
       </c>
       <c r="F133">
         <v>0.80410000000000004</v>
       </c>
       <c r="G133">
-        <v>0.15820000000000001</v>
+        <v>0.203765048732165</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -4792,16 +4799,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D134">
-        <v>-0.2359</v>
+        <v>-0.24437455454444301</v>
       </c>
       <c r="E134">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.06304864657387E-2</v>
       </c>
       <c r="F134">
         <v>0.80410000000000004</v>
       </c>
       <c r="G134">
-        <v>0.15820000000000001</v>
+        <v>0.17047041837942301</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -4815,16 +4822,16 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <v>-0.2359</v>
+        <v>-0.24437455454444301</v>
       </c>
       <c r="E135">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.06304864657387E-2</v>
       </c>
       <c r="F135">
         <v>0.80410000000000004</v>
       </c>
       <c r="G135">
-        <v>0.15820000000000001</v>
+        <v>0.17047041837942301</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -4838,16 +4845,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D136">
-        <v>-0.2359</v>
+        <v>-0.105130043924235</v>
       </c>
       <c r="E136">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.1634768493368798E-2</v>
       </c>
       <c r="F136">
         <v>0.80410000000000004</v>
       </c>
       <c r="G136">
-        <v>0.15820000000000001</v>
+        <v>0.14483721286422699</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -4861,16 +4868,16 @@
         <v>0</v>
       </c>
       <c r="D137">
-        <v>-0.2359</v>
+        <v>-0.105130043924235</v>
       </c>
       <c r="E137">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.1634768493368798E-2</v>
       </c>
       <c r="F137">
         <v>0.80410000000000004</v>
       </c>
       <c r="G137">
-        <v>0.15820000000000001</v>
+        <v>0.14483721286422699</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -4884,16 +4891,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D138">
-        <v>-0.2359</v>
+        <v>-0.28287841431732103</v>
       </c>
       <c r="E138">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.2547698403235902E-2</v>
       </c>
       <c r="F138">
         <v>0.80410000000000004</v>
       </c>
       <c r="G138">
-        <v>0.15820000000000001</v>
+        <v>0.117659892445084</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -4907,16 +4914,16 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <v>-0.2359</v>
+        <v>-0.28287841431732103</v>
       </c>
       <c r="E139">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.2547698403235902E-2</v>
       </c>
       <c r="F139">
         <v>0.80410000000000004</v>
       </c>
       <c r="G139">
-        <v>0.15820000000000001</v>
+        <v>0.117659892445084</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -4930,16 +4937,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D140">
-        <v>-0.2359</v>
+        <v>-0.14651787068073899</v>
       </c>
       <c r="E140">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.5008767621567899E-2</v>
       </c>
       <c r="F140">
         <v>0.80410000000000004</v>
       </c>
       <c r="G140">
-        <v>0.15820000000000001</v>
+        <v>7.1787740845576403E-2</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -4953,16 +4960,16 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <v>-0.2359</v>
+        <v>-0.14651787068073899</v>
       </c>
       <c r="E141">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.5008767621567899E-2</v>
       </c>
       <c r="F141">
         <v>0.80410000000000004</v>
       </c>
       <c r="G141">
-        <v>0.15820000000000001</v>
+        <v>7.1787740845576403E-2</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -4976,16 +4983,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D142">
-        <v>-0.2359</v>
+        <v>-0.21165375067513101</v>
       </c>
       <c r="E142">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.02026985190999E-2</v>
       </c>
       <c r="F142">
         <v>0.80410000000000004</v>
       </c>
       <c r="G142">
-        <v>0.15820000000000001</v>
+        <v>0.195555254956219</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -4999,16 +5006,16 @@
         <v>0</v>
       </c>
       <c r="D143">
-        <v>-0.2359</v>
+        <v>-0.21165375067513101</v>
       </c>
       <c r="E143">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.02026985190999E-2</v>
       </c>
       <c r="F143">
         <v>0.80410000000000004</v>
       </c>
       <c r="G143">
-        <v>0.15820000000000001</v>
+        <v>0.195555254956219</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -5022,16 +5029,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D144">
-        <v>-0.2359</v>
+        <v>-3.1905417305185001E-2</v>
       </c>
       <c r="E144">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.8098970887569397E-2</v>
       </c>
       <c r="F144">
         <v>0.80410000000000004</v>
       </c>
       <c r="G144">
-        <v>0.15820000000000001</v>
+        <v>0.16512702923033901</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -5045,16 +5052,16 @@
         <v>0</v>
       </c>
       <c r="D145">
-        <v>-0.2359</v>
+        <v>-3.1905417305185001E-2</v>
       </c>
       <c r="E145">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.8098970887569397E-2</v>
       </c>
       <c r="F145">
         <v>0.80410000000000004</v>
       </c>
       <c r="G145">
-        <v>0.15820000000000001</v>
+        <v>0.16512702923033901</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -5068,16 +5075,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D146">
-        <v>-0.2359</v>
+        <v>-0.367097527050112</v>
       </c>
       <c r="E146">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.43786341524682E-2</v>
       </c>
       <c r="F146">
         <v>0.80410000000000004</v>
       </c>
       <c r="G146">
-        <v>0.15820000000000001</v>
+        <v>0.139762023026136</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -5091,16 +5098,16 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <v>-0.2359</v>
+        <v>-0.367097527050112</v>
       </c>
       <c r="E147">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.43786341524682E-2</v>
       </c>
       <c r="F147">
         <v>0.80410000000000004</v>
       </c>
       <c r="G147">
-        <v>0.15820000000000001</v>
+        <v>0.139762023026136</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -5114,16 +5121,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D148">
-        <v>-0.2359</v>
+        <v>-0.18809975787064001</v>
       </c>
       <c r="E148">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.6718118024534702E-2</v>
       </c>
       <c r="F148">
         <v>0.80410000000000004</v>
       </c>
       <c r="G148">
-        <v>0.15820000000000001</v>
+        <v>0.11120093269147099</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -5137,16 +5144,16 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <v>-0.2359</v>
+        <v>-0.18809975787064001</v>
       </c>
       <c r="E149">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.6718118024534702E-2</v>
       </c>
       <c r="F149">
         <v>0.80410000000000004</v>
       </c>
       <c r="G149">
-        <v>0.15820000000000001</v>
+        <v>0.11120093269147099</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -5160,16 +5167,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D150">
-        <v>-0.2359</v>
+        <v>-0.253199918135114</v>
       </c>
       <c r="E150">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.7474838926142505E-2</v>
       </c>
       <c r="F150">
         <v>0.80410000000000004</v>
       </c>
       <c r="G150">
-        <v>0.15820000000000001</v>
+        <v>4.61274753373229E-2</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -5183,16 +5190,16 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <v>-0.2359</v>
+        <v>-0.253199918135114</v>
       </c>
       <c r="E151">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.7474838926142505E-2</v>
       </c>
       <c r="F151">
         <v>0.80410000000000004</v>
       </c>
       <c r="G151">
-        <v>0.15820000000000001</v>
+        <v>4.61274753373229E-2</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -5206,16 +5213,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D152">
-        <v>-0.2359</v>
+        <v>-0.116775990694114</v>
       </c>
       <c r="E152">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.8772850820752597E-2</v>
       </c>
       <c r="F152">
         <v>0.80410000000000004</v>
       </c>
       <c r="G152">
-        <v>0.15820000000000001</v>
+        <v>0.244694353916348</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -5229,16 +5236,16 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <v>-0.2359</v>
+        <v>-0.116775990694114</v>
       </c>
       <c r="E153">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.8772850820752597E-2</v>
       </c>
       <c r="F153">
         <v>0.80410000000000004</v>
       </c>
       <c r="G153">
-        <v>0.15820000000000001</v>
+        <v>0.244694353916348</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -5252,16 +5259,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D154">
-        <v>-0.2359</v>
+        <v>-0.29448674277758102</v>
       </c>
       <c r="E154">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.8590602626726101E-2</v>
       </c>
       <c r="F154">
         <v>0.80410000000000004</v>
       </c>
       <c r="G154">
-        <v>0.15820000000000001</v>
+        <v>0.18708740260917101</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -5275,16 +5282,16 @@
         <v>0</v>
       </c>
       <c r="D155">
-        <v>-0.2359</v>
+        <v>-0.29448674277758102</v>
       </c>
       <c r="E155">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.8590602626726101E-2</v>
       </c>
       <c r="F155">
         <v>0.80410000000000004</v>
       </c>
       <c r="G155">
-        <v>0.15820000000000001</v>
+        <v>0.18708740260917101</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -5298,16 +5305,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D156">
-        <v>-0.2359</v>
+        <v>-0.15535516826182</v>
       </c>
       <c r="E156">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.0359347730489697E-2</v>
       </c>
       <c r="F156">
         <v>0.80410000000000004</v>
       </c>
       <c r="G156">
-        <v>0.15820000000000001</v>
+        <v>0.15893075099352599</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -5321,16 +5328,16 @@
         <v>0</v>
       </c>
       <c r="D157">
-        <v>-0.2359</v>
+        <v>-0.15535516826182</v>
       </c>
       <c r="E157">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.0359347730489697E-2</v>
       </c>
       <c r="F157">
         <v>0.80410000000000004</v>
       </c>
       <c r="G157">
-        <v>0.15820000000000001</v>
+        <v>0.15893075099352599</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -5344,16 +5351,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D158">
-        <v>-0.2359</v>
+        <v>-0.21958512916095799</v>
       </c>
       <c r="E158">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.3066947597698899E-2</v>
       </c>
       <c r="F158">
         <v>0.80410000000000004</v>
       </c>
       <c r="G158">
-        <v>0.15820000000000001</v>
+        <v>0.133523822720131</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5367,16 +5374,16 @@
         <v>0</v>
       </c>
       <c r="D159">
-        <v>-0.2359</v>
+        <v>-0.21958512916095799</v>
       </c>
       <c r="E159">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.3066947597698899E-2</v>
       </c>
       <c r="F159">
         <v>0.80410000000000004</v>
       </c>
       <c r="G159">
-        <v>0.15820000000000001</v>
+        <v>0.133523822720131</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -5390,16 +5397,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D160">
-        <v>-0.2359</v>
+        <v>-5.7885096561410103E-2</v>
       </c>
       <c r="E160">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.27006047119405E-2</v>
       </c>
       <c r="F160">
         <v>0.80410000000000004</v>
       </c>
       <c r="G160">
-        <v>0.15820000000000001</v>
+        <v>0.102465326104138</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5413,16 +5420,16 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <v>-0.2359</v>
+        <v>-5.7885096561410103E-2</v>
       </c>
       <c r="E161">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.27006047119405E-2</v>
       </c>
       <c r="F161">
         <v>0.80410000000000004</v>
       </c>
       <c r="G161">
-        <v>0.15820000000000001</v>
+        <v>0.102465326104138</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5436,16 +5443,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D162">
-        <v>-0.2359</v>
+        <v>-0.32272555343398401</v>
       </c>
       <c r="E162">
-        <v>-4.8800000000000003E-2</v>
+        <v>-9.1808466447300299E-2</v>
       </c>
       <c r="F162">
         <v>0.80410000000000004</v>
       </c>
       <c r="G162">
-        <v>0.15820000000000001</v>
+        <v>0.22411885194253001</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -5459,16 +5466,16 @@
         <v>0</v>
       </c>
       <c r="D163">
-        <v>-0.2359</v>
+        <v>-0.32272555343398401</v>
       </c>
       <c r="E163">
-        <v>-4.8800000000000003E-2</v>
+        <v>-9.1808466447300299E-2</v>
       </c>
       <c r="F163">
         <v>0.80410000000000004</v>
       </c>
       <c r="G163">
-        <v>0.15820000000000001</v>
+        <v>0.22411885194253001</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5482,16 +5489,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D164">
-        <v>-0.2359</v>
+        <v>-0.17210372837868701</v>
       </c>
       <c r="E164">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7618835422117799E-2</v>
       </c>
       <c r="F164">
         <v>0.80410000000000004</v>
       </c>
       <c r="G164">
-        <v>0.15820000000000001</v>
+        <v>0.180773831372468</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5505,16 +5512,16 @@
         <v>0</v>
       </c>
       <c r="D165">
-        <v>-0.2359</v>
+        <v>-0.17210372837868701</v>
       </c>
       <c r="E165">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.7618835422117799E-2</v>
       </c>
       <c r="F165">
         <v>0.80410000000000004</v>
       </c>
       <c r="G165">
-        <v>0.15820000000000001</v>
+        <v>0.180773831372468</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5528,16 +5535,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D166">
-        <v>-0.2359</v>
+        <v>-0.23588242603676199</v>
       </c>
       <c r="E166">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.0367908540111401E-2</v>
       </c>
       <c r="F166">
         <v>0.80410000000000004</v>
       </c>
       <c r="G166">
-        <v>0.15820000000000001</v>
+        <v>0.15387410692283299</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5551,16 +5558,16 @@
         <v>0</v>
       </c>
       <c r="D167">
-        <v>-0.2359</v>
+        <v>-0.23588242603676199</v>
       </c>
       <c r="E167">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.0367908540111401E-2</v>
       </c>
       <c r="F167">
         <v>0.80410000000000004</v>
       </c>
       <c r="G167">
-        <v>0.15820000000000001</v>
+        <v>0.15387410692283299</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5574,16 +5581,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D168">
-        <v>-0.2359</v>
+        <v>-9.2029471002581797E-2</v>
       </c>
       <c r="E168">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.2584543543426194E-2</v>
       </c>
       <c r="F168">
         <v>0.80410000000000004</v>
       </c>
       <c r="G168">
-        <v>0.15820000000000001</v>
+        <v>0.128125773991704</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5597,16 +5604,16 @@
         <v>0</v>
       </c>
       <c r="D169">
-        <v>-0.2359</v>
+        <v>-9.2029471002581797E-2</v>
       </c>
       <c r="E169">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.2584543543426194E-2</v>
       </c>
       <c r="F169">
         <v>0.80410000000000004</v>
       </c>
       <c r="G169">
-        <v>0.15820000000000001</v>
+        <v>0.128125773991704</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5620,16 +5627,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D170">
-        <v>-0.2359</v>
+        <v>-0.27229240247428299</v>
       </c>
       <c r="E170">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.1870948414149999E-2</v>
       </c>
       <c r="F170">
         <v>0.80410000000000004</v>
       </c>
       <c r="G170">
-        <v>0.15820000000000001</v>
+        <v>9.3887951832412497E-2</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5643,16 +5650,16 @@
         <v>0</v>
       </c>
       <c r="D171">
-        <v>-0.2359</v>
+        <v>-0.27229240247428299</v>
       </c>
       <c r="E171">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.1870948414149999E-2</v>
       </c>
       <c r="F171">
         <v>0.80410000000000004</v>
       </c>
       <c r="G171">
-        <v>0.15820000000000001</v>
+        <v>9.3887951832412497E-2</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5666,16 +5673,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D172">
-        <v>-0.2359</v>
+        <v>-0.13724113372253499</v>
       </c>
       <c r="E172">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.3446855660491E-2</v>
       </c>
       <c r="F172">
         <v>0.80410000000000004</v>
       </c>
       <c r="G172">
-        <v>0.15820000000000001</v>
+        <v>0.21156107931759199</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5689,16 +5696,16 @@
         <v>0</v>
       </c>
       <c r="D173">
-        <v>-0.2359</v>
+        <v>-0.13724113372253499</v>
       </c>
       <c r="E173">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.3446855660491E-2</v>
       </c>
       <c r="F173">
         <v>0.80410000000000004</v>
       </c>
       <c r="G173">
-        <v>0.15820000000000001</v>
+        <v>0.21156107931759199</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5712,16 +5719,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D174">
-        <v>-0.2359</v>
+        <v>-0.20379512354064799</v>
       </c>
       <c r="E174">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4093123388004394E-2</v>
       </c>
       <c r="F174">
         <v>0.80410000000000004</v>
       </c>
       <c r="G174">
-        <v>0.15820000000000001</v>
+        <v>0.17491731353245399</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5735,16 +5742,16 @@
         <v>0</v>
       </c>
       <c r="D175">
-        <v>-0.2359</v>
+        <v>-0.20379512354064799</v>
       </c>
       <c r="E175">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.4093123388004394E-2</v>
       </c>
       <c r="F175">
         <v>0.80410000000000004</v>
       </c>
       <c r="G175">
-        <v>0.15820000000000001</v>
+        <v>0.17491731353245399</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5757,17 +5764,17 @@
       <c r="C176">
         <v>-0.3422</v>
       </c>
-      <c r="D176">
-        <v>-0.2359</v>
+      <c r="D176" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E176">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6276540065288502E-2</v>
       </c>
       <c r="F176">
         <v>0.80410000000000004</v>
       </c>
       <c r="G176">
-        <v>0.15820000000000001</v>
+        <v>0.14885687793126201</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5780,17 +5787,17 @@
       <c r="C177">
         <v>0</v>
       </c>
-      <c r="D177">
-        <v>-0.2359</v>
+      <c r="D177" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E177">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.6276540065288502E-2</v>
       </c>
       <c r="F177">
         <v>0.80410000000000004</v>
       </c>
       <c r="G177">
-        <v>0.15820000000000001</v>
+        <v>0.14885687793126201</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -5804,16 +5811,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D178">
-        <v>-0.2359</v>
+        <v>-0.43954150110677498</v>
       </c>
       <c r="E178">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.35283916644109E-2</v>
       </c>
       <c r="F178">
         <v>0.80410000000000004</v>
       </c>
       <c r="G178">
-        <v>0.15820000000000001</v>
+        <v>0.122459213503769</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -5827,16 +5834,16 @@
         <v>0</v>
       </c>
       <c r="D179">
-        <v>-0.2359</v>
+        <v>-0.43954150110677498</v>
       </c>
       <c r="E179">
-        <v>-4.8800000000000003E-2</v>
+        <v>-2.35283916644109E-2</v>
       </c>
       <c r="F179">
         <v>0.80410000000000004</v>
       </c>
       <c r="G179">
-        <v>0.15820000000000001</v>
+        <v>0.122459213503769</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -5850,16 +5857,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D180">
-        <v>-0.2359</v>
+        <v>-0.19791915254621201</v>
       </c>
       <c r="E180">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.1905221716383897E-2</v>
       </c>
       <c r="F180">
         <v>0.80410000000000004</v>
       </c>
       <c r="G180">
-        <v>0.15820000000000001</v>
+        <v>8.3232221651971597E-2</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -5873,16 +5880,16 @@
         <v>0</v>
       </c>
       <c r="D181">
-        <v>-0.2359</v>
+        <v>-0.19791915254621201</v>
       </c>
       <c r="E181">
-        <v>-4.8800000000000003E-2</v>
+        <v>-8.1905221716383897E-2</v>
       </c>
       <c r="F181">
         <v>0.80410000000000004</v>
       </c>
       <c r="G181">
-        <v>0.15820000000000001</v>
+        <v>8.3232221651971597E-2</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -5896,16 +5903,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D182">
-        <v>-0.2359</v>
+        <v>-0.26485928743304499</v>
       </c>
       <c r="E182">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5656251078420503E-2</v>
       </c>
       <c r="F182">
         <v>0.80410000000000004</v>
       </c>
       <c r="G182">
-        <v>0.15820000000000001</v>
+        <v>0.20201075259610499</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -5919,16 +5926,16 @@
         <v>0</v>
       </c>
       <c r="D183">
-        <v>-0.2359</v>
+        <v>-0.26485928743304499</v>
       </c>
       <c r="E183">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.5656251078420503E-2</v>
       </c>
       <c r="F183">
         <v>0.80410000000000004</v>
       </c>
       <c r="G183">
-        <v>0.15820000000000001</v>
+        <v>0.20201075259610499</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -5942,16 +5949,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D184">
-        <v>-0.2359</v>
+        <v>-0.12991528948550399</v>
       </c>
       <c r="E184">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8224517421911297E-2</v>
       </c>
       <c r="F184">
         <v>0.80410000000000004</v>
       </c>
       <c r="G184">
-        <v>0.15820000000000001</v>
+        <v>0.16938486865514099</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -5965,16 +5972,16 @@
         <v>0</v>
       </c>
       <c r="D185">
-        <v>-0.2359</v>
+        <v>-0.12991528948550399</v>
       </c>
       <c r="E185">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.8224517421911297E-2</v>
       </c>
       <c r="F185">
         <v>0.80410000000000004</v>
       </c>
       <c r="G185">
-        <v>0.15820000000000001</v>
+        <v>0.16938486865514099</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -5988,16 +5995,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D186">
-        <v>-0.2359</v>
+        <v>-0.311092284192306</v>
       </c>
       <c r="E186">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.9366740236045499E-2</v>
       </c>
       <c r="F186">
         <v>0.80410000000000004</v>
       </c>
       <c r="G186">
-        <v>0.15820000000000001</v>
+        <v>0.14382808310863099</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -6011,16 +6018,16 @@
         <v>0</v>
       </c>
       <c r="D187">
-        <v>-0.2359</v>
+        <v>-0.311092284192306</v>
       </c>
       <c r="E187">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.9366740236045499E-2</v>
       </c>
       <c r="F187">
         <v>0.80410000000000004</v>
       </c>
       <c r="G187">
-        <v>0.15820000000000001</v>
+        <v>0.14382808310863099</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -6034,16 +6041,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D188">
-        <v>-0.2359</v>
+        <v>-0.16593916432688699</v>
       </c>
       <c r="E188">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.0011461492509499E-2</v>
       </c>
       <c r="F188">
         <v>0.80410000000000004</v>
       </c>
       <c r="G188">
-        <v>0.15820000000000001</v>
+        <v>0.116413845579488</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -6057,16 +6064,16 @@
         <v>0</v>
       </c>
       <c r="D189">
-        <v>-0.2359</v>
+        <v>-0.16593916432688699</v>
       </c>
       <c r="E189">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.0011461492509499E-2</v>
       </c>
       <c r="F189">
         <v>0.80410000000000004</v>
       </c>
       <c r="G189">
-        <v>0.15820000000000001</v>
+        <v>0.116413845579488</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -6080,16 +6087,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D190">
-        <v>-0.2359</v>
+        <v>-0.22968231079645199</v>
       </c>
       <c r="E190">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0669861391545001E-2</v>
       </c>
       <c r="F190">
         <v>0.80410000000000004</v>
       </c>
       <c r="G190">
-        <v>0.15820000000000001</v>
+        <v>6.8180980324637097E-2</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -6103,16 +6110,16 @@
         <v>0</v>
       </c>
       <c r="D191">
-        <v>-0.2359</v>
+        <v>-0.22968231079645199</v>
       </c>
       <c r="E191">
-        <v>-4.8800000000000003E-2</v>
+        <v>-3.0669861391545001E-2</v>
       </c>
       <c r="F191">
         <v>0.80410000000000004</v>
       </c>
       <c r="G191">
-        <v>0.15820000000000001</v>
+        <v>6.8180980324637097E-2</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -6126,16 +6133,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D192">
-        <v>-0.2359</v>
+        <v>-8.0834981273203599E-2</v>
       </c>
       <c r="E192">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.1802754816183803E-2</v>
       </c>
       <c r="F192">
         <v>0.80410000000000004</v>
       </c>
       <c r="G192">
-        <v>0.15820000000000001</v>
+        <v>0.194057189353598</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -6149,16 +6156,16 @@
         <v>0</v>
       </c>
       <c r="D193">
-        <v>-0.2359</v>
+        <v>-8.0834981273203599E-2</v>
       </c>
       <c r="E193">
-        <v>-4.8800000000000003E-2</v>
+        <v>-6.1802754816183803E-2</v>
       </c>
       <c r="F193">
         <v>0.80410000000000004</v>
       </c>
       <c r="G193">
-        <v>0.15820000000000001</v>
+        <v>0.194057189353598</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -6172,16 +6179,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D194">
-        <v>-0.2359</v>
+        <v>-0.34698530320981802</v>
       </c>
       <c r="E194">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.4367603188565703E-2</v>
       </c>
       <c r="F194">
         <v>0.80410000000000004</v>
       </c>
       <c r="G194">
-        <v>0.15820000000000001</v>
+        <v>0.16408066766540599</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -6195,16 +6202,16 @@
         <v>0</v>
       </c>
       <c r="D195">
-        <v>-0.2359</v>
+        <v>-0.34698530320981802</v>
       </c>
       <c r="E195">
-        <v>-4.8800000000000003E-2</v>
+        <v>-4.4367603188565703E-2</v>
       </c>
       <c r="F195">
         <v>0.80410000000000004</v>
       </c>
       <c r="G195">
-        <v>0.15820000000000001</v>
+        <v>0.16408066766540599</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -6218,16 +6225,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D196">
-        <v>-0.2359</v>
+        <v>-0.182158674140557</v>
       </c>
       <c r="E196">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.8176336524457999E-2</v>
       </c>
       <c r="F196">
         <v>0.80410000000000004</v>
       </c>
       <c r="G196">
-        <v>0.15820000000000001</v>
+        <v>0.13873590631831301</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -6241,16 +6248,16 @@
         <v>0</v>
       </c>
       <c r="D197">
-        <v>-0.2359</v>
+        <v>-0.182158674140557</v>
       </c>
       <c r="E197">
-        <v>-4.8800000000000003E-2</v>
+        <v>-1.8176336524457999E-2</v>
       </c>
       <c r="F197">
         <v>0.80410000000000004</v>
       </c>
       <c r="G197">
-        <v>0.15820000000000001</v>
+        <v>0.13873590631831301</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -6264,16 +6271,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D198">
-        <v>-0.2359</v>
+        <v>-0.24654607164045</v>
       </c>
       <c r="E198">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.6526749577736294E-2</v>
       </c>
       <c r="F198">
         <v>0.80410000000000004</v>
       </c>
       <c r="G198">
-        <v>0.15820000000000001</v>
+        <v>0.109831421305519</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -6287,16 +6294,16 @@
         <v>0</v>
       </c>
       <c r="D199">
-        <v>-0.2359</v>
+        <v>-0.24654607164045</v>
       </c>
       <c r="E199">
-        <v>-4.8800000000000003E-2</v>
+        <v>-7.6526749577736294E-2</v>
       </c>
       <c r="F199">
         <v>0.80410000000000004</v>
       </c>
       <c r="G199">
-        <v>0.15820000000000001</v>
+        <v>0.109831421305519</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -6310,16 +6317,16 @@
         <v>-0.3422</v>
       </c>
       <c r="D200">
-        <v>-0.2359</v>
+        <v>-0.10815788793329199</v>
       </c>
       <c r="E200">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3746786178045E-2</v>
       </c>
       <c r="F200">
         <v>0.80410000000000004</v>
       </c>
       <c r="G200">
-        <v>0.15820000000000001</v>
+        <v>3.5273435603358598E-2</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -6333,16 +6340,16 @@
         <v>0</v>
       </c>
       <c r="D201">
-        <v>-0.2359</v>
+        <v>-0.10815788793329199</v>
       </c>
       <c r="E201">
-        <v>-4.8800000000000003E-2</v>
+        <v>-5.3746786178045E-2</v>
       </c>
       <c r="F201">
         <v>0.80410000000000004</v>
       </c>
       <c r="G201">
-        <v>0.15820000000000001</v>
+        <v>3.5273435603358598E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extracted duals instead of heuristic convergence
</commit_message>
<xml_diff>
--- a/MILP/Input Data/master_problem_inputs_with_taste_draws.xlsx
+++ b/MILP/Input Data/master_problem_inputs_with_taste_draws.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atfan\Desktop\M.Sc DDS\Sem 4\Master's Thesis\Code\MILP\Input Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48741B5A-EE4D-494C-AF71-A3793FC347E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574DCCBE-8A7A-4139-9C1F-BC118E0F40BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD_pairs" sheetId="1" r:id="rId1"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,26 +924,27 @@
         <v>247.95599999999999</v>
       </c>
       <c r="F2">
-        <v>396.7296</v>
+        <f>L2+(50/1)</f>
+        <v>246.7296</v>
       </c>
       <c r="G2">
         <f>1.3*L2</f>
-        <v>515.74847999999997</v>
+        <v>255.74848000000003</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L2">
-        <v>396.7296</v>
+        <v>196.7296</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -963,26 +964,27 @@
         <v>245.02775</v>
       </c>
       <c r="F3">
-        <v>392.0444</v>
+        <f t="shared" ref="F3:F17" si="0">L3+(50/1)</f>
+        <v>242.0444</v>
       </c>
       <c r="G3">
         <f>1.3*L3</f>
-        <v>509.65772000000004</v>
+        <v>249.65772000000001</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L3">
-        <v>392.0444</v>
+        <v>192.0444</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1002,26 +1004,27 @@
         <v>247.95599999999999</v>
       </c>
       <c r="F4">
-        <v>396.7296</v>
+        <f t="shared" si="0"/>
+        <v>246.7296</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="0">1.3*L4</f>
-        <v>515.74847999999997</v>
+        <f t="shared" ref="G4:G9" si="1">1.3*L4</f>
+        <v>255.74848000000003</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L4">
-        <v>396.7296</v>
+        <v>196.7296</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1041,26 +1044,27 @@
         <v>245.02775</v>
       </c>
       <c r="F5">
-        <v>392.0444</v>
+        <f t="shared" si="0"/>
+        <v>242.0444</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>509.65772000000004</v>
+        <f t="shared" si="1"/>
+        <v>249.65772000000001</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L5">
-        <v>392.0444</v>
+        <v>192.0444</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1080,26 +1084,27 @@
         <v>173.01300000000001</v>
       </c>
       <c r="F6">
-        <v>276.82080000000002</v>
+        <f t="shared" si="0"/>
+        <v>226.82079999999999</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>359.86704000000003</v>
+        <f t="shared" si="1"/>
+        <v>229.86704</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L6">
-        <v>276.82080000000002</v>
+        <v>176.82079999999999</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1119,26 +1124,27 @@
         <v>183.001</v>
       </c>
       <c r="F7">
-        <v>292.80160000000001</v>
+        <f t="shared" si="0"/>
+        <v>242.80160000000001</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>380.64208000000002</v>
+        <f t="shared" si="1"/>
+        <v>250.64208000000002</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L7">
-        <v>292.80160000000001</v>
+        <v>192.80160000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1158,26 +1164,27 @@
         <v>285.77073015873009</v>
       </c>
       <c r="F8">
-        <v>457.23316825396802</v>
+        <f t="shared" si="0"/>
+        <v>307.23316825396802</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>594.40311873015867</v>
+        <f t="shared" si="1"/>
+        <v>334.40311873015844</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L8">
-        <v>457.23316825396819</v>
+        <v>257.23316825396802</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1197,26 +1204,27 @@
         <v>284.86388834951458</v>
       </c>
       <c r="F9">
-        <v>455.78222135922329</v>
+        <f t="shared" si="0"/>
+        <v>305.782221359223</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>592.51688776699029</v>
+        <f t="shared" si="1"/>
+        <v>332.5168877669899</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="J9">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1500</v>
+        <v>50</v>
       </c>
       <c r="L9">
-        <v>455.78222135922329</v>
+        <v>255.782221359223</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1236,7 +1244,8 @@
         <v>247.95599999999999</v>
       </c>
       <c r="F10">
-        <v>155.63758000000001</v>
+        <f t="shared" si="0"/>
+        <v>205.63758000000001</v>
       </c>
       <c r="G10">
         <f>1.6*L10</f>
@@ -1275,10 +1284,11 @@
         <v>245.02775</v>
       </c>
       <c r="F11">
-        <v>155.47652625000001</v>
+        <f t="shared" si="0"/>
+        <v>205.47652625000001</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G17" si="1">1.6*L11</f>
+        <f t="shared" ref="G11:G17" si="2">1.6*L11</f>
         <v>248.76244200000002</v>
       </c>
       <c r="H11">
@@ -1314,10 +1324,11 @@
         <v>247.95599999999999</v>
       </c>
       <c r="F12">
-        <v>155.63758000000001</v>
+        <f t="shared" si="0"/>
+        <v>205.63758000000001</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>249.02012800000003</v>
       </c>
       <c r="H12">
@@ -1353,10 +1364,11 @@
         <v>245.02775</v>
       </c>
       <c r="F13">
-        <v>155.47652625000001</v>
+        <f t="shared" si="0"/>
+        <v>205.47652625000001</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248.76244200000002</v>
       </c>
       <c r="H13">
@@ -1392,10 +1404,11 @@
         <v>173.01300000000001</v>
       </c>
       <c r="F14">
-        <v>151.515715</v>
+        <f t="shared" si="0"/>
+        <v>201.515715</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>242.42514400000002</v>
       </c>
       <c r="H14">
@@ -1431,10 +1444,11 @@
         <v>183.001</v>
       </c>
       <c r="F15">
-        <v>152.065055</v>
+        <f t="shared" si="0"/>
+        <v>202.065055</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>243.30408800000001</v>
       </c>
       <c r="H15">
@@ -1470,10 +1484,11 @@
         <v>285.77073015873009</v>
       </c>
       <c r="F16">
-        <v>157.71739015873021</v>
+        <f t="shared" si="0"/>
+        <v>207.71739015873021</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252.34782425396835</v>
       </c>
       <c r="H16">
@@ -1509,10 +1524,11 @@
         <v>284.86388834951458</v>
       </c>
       <c r="F17">
-        <v>157.66751385922331</v>
+        <f t="shared" si="0"/>
+        <v>207.66751385922331</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252.26802217475731</v>
       </c>
       <c r="H17">
@@ -1714,7 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>

</xml_diff>